<commit_message>
Se obtiene señal resultante efectiva, comienza etapa de diseño del sistema
</commit_message>
<xml_diff>
--- a/MedicionesYMuestras/TarjetaSMA.xlsx
+++ b/MedicionesYMuestras/TarjetaSMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8550f0b6c01ec0ad/Documentos/003_laboratorioCAF/0021_placaConvertidor/MedicionesYMuestras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="700" documentId="11_AD4D2F04E46CFB4ACB3E20EE8516F1FC693EDF1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B78C4AD3-9638-4742-A3DD-E2C8ADAE8626}"/>
+  <xr:revisionPtr revIDLastSave="718" documentId="11_AD4D2F04E46CFB4ACB3E20EE8516F1FC693EDF1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78DEBB7F-19CE-40A2-B65C-F97080EE4563}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="64">
   <si>
     <t>PIN</t>
   </si>
@@ -220,13 +220,22 @@
   </si>
   <si>
     <t>Q20.4</t>
+  </si>
+  <si>
+    <t>Q20.11</t>
+  </si>
+  <si>
+    <t>Q23.9</t>
+  </si>
+  <si>
+    <t>INVERSOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +247,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -579,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -650,7 +667,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -663,9 +695,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -674,29 +703,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,42 +1047,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="45" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="35" t="s">
+      <c r="L1" s="30"/>
+      <c r="M1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1087,16 +1107,16 @@
       <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -1257,7 +1277,7 @@
       <c r="I6" s="10">
         <v>644.79999999999995</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="43" t="s">
         <v>54</v>
       </c>
       <c r="K6" s="12">
@@ -1272,7 +1292,7 @@
       <c r="N6" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="O6" s="40" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1304,7 +1324,7 @@
       <c r="I7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="43" t="s">
         <v>55</v>
       </c>
       <c r="K7" s="12">
@@ -1319,7 +1339,7 @@
       <c r="N7" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="O7" s="37"/>
+      <c r="O7" s="41"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1493,7 +1513,7 @@
       <c r="N11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="O11" s="31" t="s">
+      <c r="O11" s="36" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1540,7 +1560,7 @@
       <c r="N12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="32"/>
+      <c r="O12" s="37"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1585,7 +1605,7 @@
       <c r="N13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="32"/>
+      <c r="O13" s="37"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -1630,7 +1650,7 @@
       <c r="N14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O14" s="32"/>
+      <c r="O14" s="37"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1675,7 +1695,7 @@
       <c r="N15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="32"/>
+      <c r="O15" s="37"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -1718,7 +1738,7 @@
         <v>40</v>
       </c>
       <c r="N16" s="6"/>
-      <c r="O16" s="32"/>
+      <c r="O16" s="37"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -1761,7 +1781,7 @@
         <v>38</v>
       </c>
       <c r="N17" s="6"/>
-      <c r="O17" s="32"/>
+      <c r="O17" s="37"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -1806,7 +1826,7 @@
       <c r="N18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="32"/>
+      <c r="O18" s="37"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -1851,9 +1871,9 @@
       <c r="N19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="O19" s="33"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O19" s="38"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1888,9 +1908,9 @@
       <c r="L20" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -1920,18 +1940,26 @@
       <c r="I21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="J21" s="42" t="s">
+        <v>54</v>
+      </c>
       <c r="K21" s="12">
         <v>3.97</v>
       </c>
-      <c r="L21" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="O21" s="40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -1959,16 +1987,22 @@
       <c r="I22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="J22" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="K22" s="12">
         <v>0</v>
       </c>
-      <c r="L22" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22" s="1"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="L22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="O22" s="41"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2005,9 +2039,9 @@
       <c r="L23" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -2121,7 +2155,7 @@
       <c r="I26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="38" t="s">
+      <c r="J26" s="44" t="s">
         <v>53</v>
       </c>
       <c r="K26" s="12">
@@ -2166,7 +2200,7 @@
       <c r="I27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="39"/>
+      <c r="J27" s="45"/>
       <c r="K27" s="12">
         <v>0</v>
       </c>
@@ -2174,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>57</v>
@@ -2209,7 +2243,7 @@
       <c r="I28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="39"/>
+      <c r="J28" s="45"/>
       <c r="K28" s="12">
         <v>0</v>
       </c>
@@ -2217,7 +2251,7 @@
         <v>2</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="N28" s="6" t="s">
         <v>58</v>
@@ -2252,7 +2286,7 @@
       <c r="I29" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="40"/>
+      <c r="J29" s="46"/>
       <c r="K29" s="12">
         <v>0</v>
       </c>
@@ -2311,7 +2345,13 @@
       <c r="O30" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="O11:O19"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="O6:O7"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="J26:J29"/>
     <mergeCell ref="B1:C1"/>
@@ -2320,11 +2360,6 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="O11:O19"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="O6:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="J30:J1048576 J1:J26">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="CONSTANTE">
@@ -2360,33 +2395,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="45" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="45"/>
+      <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2411,7 +2446,7 @@
       <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="12" t="s">
         <v>1</v>
       </c>

</xml_diff>